<commit_message>
bite rate per wave energy for bejarano sp
</commit_message>
<xml_diff>
--- a/data/herb_biterate_estimates.xlsx
+++ b/data/herb_biterate_estimates.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="24">
   <si>
     <t>Calotomus carolinus</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">wave energy = </t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -93,6 +90,15 @@
   </si>
   <si>
     <t>James</t>
+  </si>
+  <si>
+    <t>medium wave</t>
+  </si>
+  <si>
+    <t>high wave</t>
+  </si>
+  <si>
+    <t>low wave</t>
   </si>
 </sst>
 </file>
@@ -128,8 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,10 +442,10 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -444,145 +453,412 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6.25</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8.6111111111111107</v>
+      </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1">
+        <v>19.2053264604811</v>
+      </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.9660652920962201</v>
+      </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10.95505617977528</v>
+      </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1">
+        <v>37.604215048377434</v>
+      </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.1235955056179774</v>
+      </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>2.7083333333333335</v>
+      </c>
       <c r="E9" t="s">
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <v>35.799934832192896</v>
+      </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1">
+        <v>31.365629984051036</v>
+      </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1">
+        <v>33.463622776152754</v>
+      </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7.2330934173039436</v>
+      </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1">
+        <v>328.12092005062789</v>
+      </c>
       <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1">
+        <v>253.73992677916567</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.4016064257028118</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1">
+        <v>18.166035353535349</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1">
+        <v>21.521416083916083</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1">
+        <v>10.464456391875746</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1">
+        <v>4.7422680412371134</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1">
+        <v>9.3862007168458792</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1">
+        <v>40.889554611745936</v>
+      </c>
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
         <v>21</v>
+      </c>
+      <c r="D24" s="1">
+        <v>29.112461647740066</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1">
+        <v>18.765962307496867</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added bellwood choat species
</commit_message>
<xml_diff>
--- a/data/herb_biterate_estimates.xlsx
+++ b/data/herb_biterate_estimates.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="67">
   <si>
     <t>Calotomus carolinus</t>
   </si>
@@ -102,19 +102,150 @@
   </si>
   <si>
     <t>bites per hour per m^2</t>
+  </si>
+  <si>
+    <t>Bellwood_Choat</t>
+  </si>
+  <si>
+    <t>bites per hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolbometopon muricatum </t>
+  </si>
+  <si>
+    <t>Chlorurus bleekeri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparisoma axillare </t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>Scarus cretense</t>
+  </si>
+  <si>
+    <t>Scarus flavipectoralis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus frondosum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus ghobban </t>
+  </si>
+  <si>
+    <t>Scarus globiceps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus iseri </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus niger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus psittacus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus rivulatus </t>
+  </si>
+  <si>
+    <t>Scarus rubroviolaceus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus schlegeli </t>
+  </si>
+  <si>
+    <t>Scarus spinus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus tuiupiranga </t>
+  </si>
+  <si>
+    <t>Scarus vetula</t>
+  </si>
+  <si>
+    <t>Scarus zelindae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus frenatus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorurus microrhinos </t>
+  </si>
+  <si>
+    <t>Chlorurus ocellatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chlorurus spilurus </t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>bites per hour per m^3</t>
+  </si>
+  <si>
+    <t>bites per hour per m^4</t>
+  </si>
+  <si>
+    <t>bites per hour per m^5</t>
+  </si>
+  <si>
+    <t>bites per hour per m^6</t>
+  </si>
+  <si>
+    <t>bites per hour per m^7</t>
+  </si>
+  <si>
+    <t>bites per hour per m^8</t>
+  </si>
+  <si>
+    <t>bites per hour per m^9</t>
+  </si>
+  <si>
+    <t>bites per hour per m^10</t>
+  </si>
+  <si>
+    <t>bites per hour per m^11</t>
+  </si>
+  <si>
+    <t>bites per hour per m^12</t>
+  </si>
+  <si>
+    <t>bites per hour per m^13</t>
+  </si>
+  <si>
+    <t>bites per hour per m^14</t>
+  </si>
+  <si>
+    <t>bites per hour per m^15</t>
+  </si>
+  <si>
+    <t>bites per hour per m^16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,11 +268,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,523 +551,1149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+    <col min="1" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1">
         <v>6.25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1">
         <v>8.6111111111111107</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1">
         <v>19.2053264604811</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1">
         <v>2.9660652920962201</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1">
         <v>10.95505617977528</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1">
         <v>37.604215048377434</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1">
         <v>1.1235955056179774</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1">
         <v>2.7083333333333335</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1">
         <v>35.799934832192896</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1">
         <v>31.365629984051036</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1">
         <v>33.463622776152754</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1">
         <v>7.2330934173039436</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1">
         <v>328.12092005062789</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1">
         <v>253.73992677916567</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>4</v>
       </c>
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="1">
         <v>6.4016064257028118</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>4</v>
       </c>
-      <c r="F16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="1">
         <v>18.166035353535349</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>7</v>
       </c>
-      <c r="F17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="1">
         <v>21.521416083916083</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>7</v>
       </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="1">
         <v>10.464456391875746</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>7</v>
       </c>
-      <c r="F19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="1">
         <v>0.55555555555555558</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>9</v>
       </c>
-      <c r="F20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
         <v>21</v>
       </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1">
         <v>4.7422680412371134</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>9</v>
       </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1">
         <v>9.3862007168458792</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>9</v>
       </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
       <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1">
         <v>40.889554611745936</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>10</v>
       </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
         <v>21</v>
       </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="1">
         <v>29.112461647740066</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>10</v>
       </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
       <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1">
         <v>18.765962307496867</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>10</v>
       </c>
-      <c r="F25" t="s">
-        <v>20</v>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="G26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="F26:F58">
+    <sortCondition ref="F26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
second half Bejarano values added to herb_biterate_estimates.xlxs
</commit_message>
<xml_diff>
--- a/data/herb_biterate_estimates.xlsx
+++ b/data/herb_biterate_estimates.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robins64/Documents/git_repos/grazing-gradients/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan-Claas\Box Sync\PhD Feedbacks\Git Repository\grazing-gradients\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E89B1E-C151-419C-A4BE-9FF525B426B7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27760" yWindow="1620" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="-27765" yWindow="1620" windowWidth="27765" windowHeight="16380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="58">
   <si>
     <t>Calotomus carolinus</t>
   </si>
@@ -188,52 +189,25 @@
     <t>Jan</t>
   </si>
   <si>
-    <t>bites per hour per m^3</t>
-  </si>
-  <si>
-    <t>bites per hour per m^4</t>
-  </si>
-  <si>
-    <t>bites per hour per m^5</t>
-  </si>
-  <si>
-    <t>bites per hour per m^6</t>
-  </si>
-  <si>
-    <t>bites per hour per m^7</t>
-  </si>
-  <si>
-    <t>bites per hour per m^8</t>
-  </si>
-  <si>
-    <t>bites per hour per m^9</t>
-  </si>
-  <si>
-    <t>bites per hour per m^10</t>
-  </si>
-  <si>
-    <t>bites per hour per m^11</t>
-  </si>
-  <si>
-    <t>bites per hour per m^12</t>
-  </si>
-  <si>
-    <t>bites per hour per m^13</t>
-  </si>
-  <si>
-    <t>bites per hour per m^14</t>
-  </si>
-  <si>
-    <t>bites per hour per m^15</t>
-  </si>
-  <si>
-    <t>bites per hour per m^16</t>
+    <t>Scarus psittacus</t>
+  </si>
+  <si>
+    <t>Siganus puellus</t>
+  </si>
+  <si>
+    <t>Siganus punctatus</t>
+  </si>
+  <si>
+    <t>Scarus schlegeli</t>
+  </si>
+  <si>
+    <t>Siganus vulpinus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -276,13 +250,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -550,22 +527,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D40"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="37.6640625" customWidth="1"/>
+    <col min="1" max="2" width="37.625" customWidth="1"/>
     <col min="3" max="3" width="28.5" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="6" max="6" width="30.1640625" customWidth="1"/>
+    <col min="6" max="6" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -588,7 +565,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -611,7 +588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -634,7 +611,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -657,7 +634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -680,7 +657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -703,7 +680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -726,7 +703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -749,7 +726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -772,7 +749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -795,7 +772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -818,7 +795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -841,7 +818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -864,7 +841,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -887,7 +864,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -910,7 +887,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -933,7 +910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -956,7 +933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -979,7 +956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1002,7 +979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1002,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1049,7 +1026,7 @@
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1073,7 +1050,7 @@
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1097,7 +1074,7 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1120,7 +1097,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -1143,555 +1120,781 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
       <c r="B26" t="s">
         <v>31</v>
       </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
       <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1">
+        <v>1.1235955056179774</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
       <c r="G26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
       <c r="B27" t="s">
         <v>31</v>
       </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
       <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1">
+        <v>16.256759113901971</v>
+      </c>
+      <c r="F27" t="s">
         <v>53</v>
       </c>
       <c r="G27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>24</v>
+      </c>
+      <c r="E28" s="1">
+        <v>77.205040091638026</v>
+      </c>
+      <c r="F28" t="s">
+        <v>53</v>
       </c>
       <c r="G28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
       </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>24</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="F29" t="s">
+        <v>54</v>
       </c>
       <c r="G29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
       </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
       <c r="D30" t="s">
-        <v>56</v>
+        <v>24</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3.4090909090909092</v>
+      </c>
+      <c r="F30" t="s">
+        <v>55</v>
       </c>
       <c r="G30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
       </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>24</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2.9166666666666665</v>
+      </c>
+      <c r="F31" t="s">
+        <v>55</v>
       </c>
       <c r="G31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>24</v>
+      </c>
+      <c r="E32" s="1">
+        <v>28.886786509972211</v>
+      </c>
+      <c r="F32" t="s">
+        <v>56</v>
       </c>
       <c r="G32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>24</v>
+      </c>
+      <c r="E33" s="1">
+        <v>18.909698840254396</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
       </c>
       <c r="G33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
       <c r="B34" t="s">
         <v>31</v>
       </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>24</v>
+      </c>
+      <c r="E34" s="1">
+        <v>152.53045605446582</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
       </c>
       <c r="G34" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>
       </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>24</v>
+      </c>
+      <c r="E35" s="1">
+        <v>14.166666666666668</v>
+      </c>
+      <c r="F35" t="s">
+        <v>44</v>
       </c>
       <c r="G35" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
       <c r="B36" t="s">
         <v>31</v>
       </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
       <c r="D36" t="s">
-        <v>62</v>
+        <v>24</v>
+      </c>
+      <c r="E36" s="1">
+        <v>103.98518445839875</v>
+      </c>
+      <c r="F36" t="s">
+        <v>44</v>
       </c>
       <c r="G36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
       <c r="B37" t="s">
         <v>31</v>
       </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>24</v>
+      </c>
+      <c r="E37" s="1">
+        <v>221.11810949087476</v>
+      </c>
+      <c r="F37" t="s">
+        <v>44</v>
       </c>
       <c r="G37" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="B38" t="s">
         <v>31</v>
       </c>
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>24</v>
+      </c>
+      <c r="E38" s="1">
+        <v>5.0493986254295535</v>
+      </c>
+      <c r="F38" t="s">
+        <v>57</v>
       </c>
       <c r="G38" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>15</v>
       </c>
       <c r="B39" t="s">
         <v>31</v>
       </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
       <c r="D39" t="s">
-        <v>65</v>
+        <v>24</v>
+      </c>
+      <c r="E39" s="1">
+        <v>18.315217391304348</v>
+      </c>
+      <c r="F39" t="s">
+        <v>57</v>
       </c>
       <c r="G39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
       <c r="B40" t="s">
         <v>31</v>
       </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
       <c r="D40" t="s">
-        <v>66</v>
+        <v>24</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F40" t="s">
+        <v>57</v>
       </c>
       <c r="G40" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="1">
+        <v>328.12092005062789</v>
+      </c>
+      <c r="F41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="1">
+        <v>253.73992677916567</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6.4016064257028118</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E44" s="1">
+        <v>19.2053264604811</v>
+      </c>
+      <c r="F44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" s="2" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" s="2" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="2" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" s="2" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" t="s">
-        <v>32</v>
-      </c>
-      <c r="D46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="2" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" s="2" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" t="s">
-        <v>32</v>
-      </c>
-      <c r="D48" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" s="2" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" t="s">
-        <v>32</v>
-      </c>
-      <c r="D49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" s="2" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" t="s">
-        <v>32</v>
-      </c>
-      <c r="D50" t="s">
-        <v>26</v>
-      </c>
-      <c r="F50" s="2" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" t="s">
+        <v>32</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" t="s">
-        <v>26</v>
-      </c>
-      <c r="F51" s="2" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>25</v>
-      </c>
-      <c r="B52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" t="s">
-        <v>26</v>
-      </c>
-      <c r="F52" s="2" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" t="s">
-        <v>26</v>
-      </c>
-      <c r="F53" s="2" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>25</v>
-      </c>
-      <c r="B54" t="s">
-        <v>32</v>
-      </c>
-      <c r="D54" t="s">
-        <v>26</v>
-      </c>
-      <c r="F54" s="2" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" t="s">
-        <v>26</v>
-      </c>
-      <c r="F55" s="2" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" t="s">
-        <v>32</v>
-      </c>
-      <c r="D56" t="s">
-        <v>26</v>
-      </c>
-      <c r="F56" s="2" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>25</v>
-      </c>
-      <c r="B57" t="s">
-        <v>32</v>
-      </c>
-      <c r="D57" t="s">
-        <v>26</v>
-      </c>
-      <c r="F57" s="2" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-      <c r="D58" t="s">
-        <v>26</v>
-      </c>
-      <c r="F58" s="2" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" t="s">
-        <v>32</v>
-      </c>
-      <c r="D59" t="s">
-        <v>26</v>
-      </c>
-      <c r="F59" s="2" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" t="s">
-        <v>32</v>
-      </c>
-      <c r="D60" t="s">
-        <v>26</v>
-      </c>
-      <c r="F60" s="2" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" t="s">
-        <v>26</v>
-      </c>
-      <c r="F61" s="2" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>25</v>
-      </c>
-      <c r="B62" t="s">
-        <v>32</v>
-      </c>
-      <c r="D62" t="s">
-        <v>26</v>
-      </c>
-      <c r="F62" s="2" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>25</v>
-      </c>
-      <c r="B63" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" t="s">
-        <v>26</v>
-      </c>
-      <c r="F63" s="2" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>25</v>
-      </c>
-      <c r="B64" t="s">
-        <v>32</v>
-      </c>
-      <c r="D64" t="s">
-        <v>26</v>
-      </c>
-      <c r="F64" s="2" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="F26:F58">
+  <sortState ref="F26:F62">
     <sortCondition ref="F26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>